<commit_message>
progress for 4/10--cleaned code, added bins/percentile ranges to histograms
</commit_message>
<xml_diff>
--- a/Dataset Status.xlsx
+++ b/Dataset Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Research\growth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD0D8436-B92E-4C55-991C-6F6EBFF5CDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A921BCB8-49C0-4E88-BA4E-8612FC030D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Basis</t>
   </si>
   <si>
-    <t>Cross-sectional/Cumulative</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -765,9 +762,6 @@
     <t>takes a long time to run reformat_excel_dates_as_row_second_index</t>
   </si>
   <si>
-    <t>need to redownload original dataset</t>
-  </si>
-  <si>
     <t>~9000</t>
   </si>
   <si>
@@ -775,13 +769,19 @@
   </si>
   <si>
     <t>double check output</t>
+  </si>
+  <si>
+    <t>~8500</t>
+  </si>
+  <si>
+    <t>Cross-sectional/ Cumulative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -812,6 +812,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -856,7 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -870,7 +878,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
@@ -895,12 +902,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1178,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,1531 +1227,1535 @@
     <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.90625" customWidth="1"/>
-    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="20" customWidth="1"/>
     <col min="7" max="7" width="23.1796875" customWidth="1"/>
     <col min="8" max="8" width="82.08984375" customWidth="1"/>
-    <col min="9" max="9" width="40.7265625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="50" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7265625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="50" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7265625" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" s="14" t="s">
+      <c r="I1" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="L1" t="s">
-        <v>233</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
+      <c r="J1" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
+        <v>96</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="K2" s="14">
-        <v>83793</v>
+        <v>98</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="13">
+        <v>46928</v>
       </c>
       <c r="L2" t="s">
-        <v>235</v>
-      </c>
-      <c r="M2" s="7"/>
+        <v>236</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
+      <c r="F3" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="K3" s="14">
-        <v>32273</v>
+        <v>65</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K3" s="13">
+        <v>11520</v>
       </c>
       <c r="L3" t="s">
         <v>235</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
+      <c r="F4" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="K4" s="14">
-        <v>63290</v>
+        <v>61</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K4" s="13">
+        <v>10813</v>
       </c>
       <c r="L4" t="s">
         <v>235</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
+      <c r="F5" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>157</v>
-      </c>
-      <c r="K5" s="15">
-        <v>37614</v>
+        <v>54</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K5" s="13">
+        <v>10118</v>
       </c>
       <c r="L5" t="s">
         <v>235</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
+      <c r="F6" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="K6" s="14">
-        <v>79388</v>
+        <v>64</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="K6" s="13">
+        <v>9927</v>
       </c>
       <c r="L6" t="s">
         <v>235</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
+      <c r="F7" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>26</v>
+        <v>99</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="K7" s="13">
+        <v>8405</v>
+      </c>
+      <c r="L7" t="s">
+        <v>236</v>
       </c>
       <c r="M7" t="s">
-        <v>30</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="K8" s="14">
-        <v>13301</v>
+        <v>109</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K8" s="13">
+        <v>24158</v>
       </c>
       <c r="L8" t="s">
-        <v>236</v>
-      </c>
-      <c r="M8" t="s">
-        <v>92</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="K9" s="14">
-        <v>11235</v>
+        <v>108</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K9" s="13">
+        <v>7462</v>
       </c>
       <c r="L9" t="s">
-        <v>236</v>
-      </c>
-      <c r="M9" t="s">
-        <v>29</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>34</v>
-      </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="K10" s="14">
-        <v>35539</v>
+        <v>117</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="K10" s="13">
+        <v>30672</v>
       </c>
       <c r="L10" t="s">
-        <v>236</v>
-      </c>
-      <c r="M10" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="K11" s="14">
-        <v>35558</v>
+      <c r="K11" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="L11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
       <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="K12" s="14">
-        <v>24158</v>
+        <v>49</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K12" s="13">
+        <v>30309</v>
       </c>
       <c r="L12" t="s">
         <v>235</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>242</v>
+      <c r="I13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K13" s="13">
+        <v>24158</v>
       </c>
       <c r="L13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>34</v>
-      </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="K14" s="14">
-        <v>30309</v>
+      <c r="I14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K14" s="13">
+        <v>12898</v>
       </c>
       <c r="L14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="K15" s="14">
-        <v>12898</v>
+        <v>57</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K15" s="13">
+        <v>10074</v>
       </c>
       <c r="L15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>34</v>
-      </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="K16" s="14">
-        <v>10118</v>
+        <v>133</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>243</v>
       </c>
       <c r="L16" t="s">
         <v>236</v>
-      </c>
-      <c r="M16" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="K17" s="14">
-        <v>10074</v>
+        <v>141</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K17" s="13">
+        <v>18836</v>
       </c>
       <c r="L17" t="s">
         <v>236</v>
-      </c>
-      <c r="M17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="K18" s="14">
-        <v>10813</v>
+      <c r="I18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="K18" s="13">
+        <v>83793</v>
       </c>
       <c r="L18" t="s">
-        <v>236</v>
-      </c>
-      <c r="M18" t="s">
-        <v>29</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="K19" s="14">
-        <v>9927</v>
+        <v>22</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K19" s="13">
+        <v>79388</v>
       </c>
       <c r="L19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K20" s="13">
+        <v>63290</v>
+      </c>
+      <c r="L20" t="s">
+        <v>234</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>156</v>
+      </c>
+      <c r="K21" s="14">
+        <v>37614</v>
+      </c>
+      <c r="L21" t="s">
+        <v>234</v>
+      </c>
+      <c r="M21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="K22" s="13">
+        <v>32273</v>
+      </c>
+      <c r="L22" t="s">
+        <v>234</v>
+      </c>
+      <c r="M22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="4"/>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="K20" s="14">
-        <v>11520</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="G23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="K23" s="13">
+        <v>4352</v>
+      </c>
+      <c r="L23" t="s">
         <v>236</v>
       </c>
-      <c r="M20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" t="s">
-        <v>72</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" t="s">
-        <v>77</v>
-      </c>
-      <c r="H22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="J22" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="2"/>
-      <c r="M22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="J23" t="s">
-        <v>29</v>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="3" t="s">
-        <v>80</v>
+      <c r="M23" s="4" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="H24" t="s">
-        <v>84</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>230</v>
+        <v>120</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="K24" s="13">
+        <v>3188</v>
+      </c>
+      <c r="L24" t="s">
+        <v>238</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E25" t="s">
-        <v>227</v>
-      </c>
-      <c r="F25" t="s">
-        <v>34</v>
-      </c>
       <c r="G25" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="H25" t="s">
-        <v>89</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="K25" s="14">
-        <v>518</v>
-      </c>
-      <c r="L25" t="s">
-        <v>237</v>
-      </c>
-      <c r="M25" s="5" t="s">
-        <v>241</v>
+        <v>139</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K25" s="13">
+        <v>2563</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E26" t="s">
-        <v>227</v>
-      </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="H26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="K26" s="14">
-        <v>9972</v>
-      </c>
-      <c r="L26" t="s">
-        <v>237</v>
+        <v>123</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="K26" s="13">
+        <v>2431</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="D27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" t="s">
-        <v>34</v>
-      </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="H27" t="s">
-        <v>99</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="K27" s="14">
-        <v>46928</v>
+        <v>128</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="K27" s="13">
+        <v>7378</v>
       </c>
       <c r="L27" t="s">
-        <v>237</v>
+        <v>241</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>34</v>
-      </c>
       <c r="G28" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>100</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="K28" s="14">
-        <v>8405</v>
+        <v>39</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K28" s="13">
+        <v>35558</v>
       </c>
       <c r="L28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M28" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" t="s">
-        <v>34</v>
-      </c>
       <c r="G29" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="H29" t="s">
-        <v>109</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="K29" s="14">
-        <v>7462</v>
+        <v>37</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="K29" s="13">
+        <v>35539</v>
       </c>
       <c r="L29" t="s">
-        <v>238</v>
+        <v>235</v>
+      </c>
+      <c r="M29" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E30" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" t="s">
-        <v>34</v>
-      </c>
       <c r="G30" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K30" s="14">
-        <v>24158</v>
+        <v>30</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="K30" s="13">
+        <v>13301</v>
       </c>
       <c r="L30" t="s">
-        <v>238</v>
+        <v>235</v>
+      </c>
+      <c r="M30" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="6"/>
+      <c r="A31" s="4"/>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E31" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" t="s">
-        <v>34</v>
-      </c>
       <c r="G31" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>240</v>
+        <v>137</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K31" s="13">
+        <v>2563</v>
+      </c>
+      <c r="L31" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E32" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G32" t="s">
-        <v>77</v>
-      </c>
-      <c r="H32" t="s">
-        <v>118</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="K32" s="14">
-        <v>30672</v>
+      <c r="J32" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K32" s="13">
+        <v>11235</v>
       </c>
       <c r="L32" t="s">
-        <v>239</v>
-      </c>
-      <c r="M32" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="M32" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>226</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" t="s">
         <v>88</v>
       </c>
-      <c r="C33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" t="s">
-        <v>122</v>
-      </c>
-      <c r="H33" t="s">
-        <v>121</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K33" s="14">
-        <v>3188</v>
+      <c r="I33" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="K33" s="13">
+        <v>9975</v>
       </c>
       <c r="L33" t="s">
-        <v>239</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>244</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F34" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" t="s">
-        <v>34</v>
-      </c>
       <c r="G34" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="H34" t="s">
-        <v>124</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="J34" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="K34" s="13">
+        <v>9972</v>
+      </c>
+      <c r="L34" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="6"/>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" t="s">
+        <v>113</v>
+      </c>
+      <c r="H35" t="s">
+        <v>114</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J35" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="K34" s="14">
-        <v>2431</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
-      <c r="B35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" t="s">
-        <v>120</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="M35" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="6"/>
+      <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" t="s">
-        <v>122</v>
-      </c>
-      <c r="H35" t="s">
-        <v>140</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="K35" s="14">
-        <v>2563</v>
-      </c>
-      <c r="M35" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
-      <c r="B36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="G36" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="5"/>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="5"/>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" t="s">
-        <v>126</v>
-      </c>
-      <c r="H36" t="s">
-        <v>127</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="K36" s="14">
-        <v>4352</v>
-      </c>
-      <c r="L36" t="s">
-        <v>237</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="4"/>
-      <c r="B37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" t="s">
-        <v>131</v>
-      </c>
-      <c r="H37" t="s">
-        <v>129</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="K37" s="14">
-        <v>7378</v>
-      </c>
-      <c r="L37" t="s">
-        <v>243</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="4"/>
-      <c r="B38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" t="s">
-        <v>135</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="G38" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J38" t="s">
+        <v>28</v>
+      </c>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" s="5"/>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E38" t="s">
-        <v>106</v>
-      </c>
-      <c r="F38" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" t="s">
-        <v>77</v>
-      </c>
-      <c r="H38" t="s">
-        <v>134</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="L38" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
-      <c r="B39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="G39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J39" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="1"/>
+      <c r="L39" s="2"/>
+      <c r="M39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="5"/>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E39" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" t="s">
-        <v>34</v>
-      </c>
-      <c r="G39" t="s">
-        <v>137</v>
-      </c>
-      <c r="H39" t="s">
-        <v>138</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="K39" s="14">
-        <v>2563</v>
-      </c>
-      <c r="L39" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="4"/>
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" t="s">
-        <v>97</v>
-      </c>
-      <c r="F40" t="s">
-        <v>34</v>
-      </c>
       <c r="G40" t="s">
-        <v>77</v>
-      </c>
-      <c r="H40" t="s">
-        <v>142</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="K40" s="14">
-        <v>18836</v>
-      </c>
-      <c r="L40" t="s">
-        <v>237</v>
+        <v>76</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J40" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M40">
+    <sortCondition sortBy="cellColor" ref="A2:A40" dxfId="1"/>
+    <sortCondition ref="C2:C40"/>
+    <sortCondition descending="1" ref="K2:K40"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="I21" r:id="rId1" xr:uid="{8EFD3ED9-6366-46E2-9654-016F042DEAF1}"/>
-    <hyperlink ref="I22" r:id="rId2" xr:uid="{5B3A061C-C2C9-487C-B6BB-2BA58CD27151}"/>
-    <hyperlink ref="I23" r:id="rId3" xr:uid="{2EB82B32-E7AF-49FC-820C-BAE52D7AAFFC}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{09CF4575-C31A-432C-8C81-0B59D8961159}"/>
+    <hyperlink ref="I38" r:id="rId1" xr:uid="{8EFD3ED9-6366-46E2-9654-016F042DEAF1}"/>
+    <hyperlink ref="I39" r:id="rId2" xr:uid="{5B3A061C-C2C9-487C-B6BB-2BA58CD27151}"/>
+    <hyperlink ref="I40" r:id="rId3" xr:uid="{2EB82B32-E7AF-49FC-820C-BAE52D7AAFFC}"/>
+    <hyperlink ref="I21" r:id="rId4" xr:uid="{09CF4575-C31A-432C-8C81-0B59D8961159}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -2724,338 +2766,338 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8C11AD-40BC-418A-885D-8177B6B4BB66}">
   <dimension ref="A1:A67"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>178</v>
+      <c r="A1" s="12" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>182</v>
+      <c r="A2" s="10" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>116</v>
+      <c r="A4" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
-        <v>179</v>
+      <c r="A21" s="12" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
-        <v>182</v>
+      <c r="A22" s="10" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
-        <v>192</v>
+      <c r="A24" s="10" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>116</v>
+      <c r="A27" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13" t="s">
-        <v>180</v>
+      <c r="A35" s="12" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
-        <v>182</v>
+      <c r="A36" s="10" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
-        <v>116</v>
+      <c r="A38" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
-        <v>194</v>
+      <c r="A41" s="10" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="10" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="11" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="12"/>
+      <c r="A46" s="11"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="13" t="s">
-        <v>181</v>
+      <c r="A47" s="12" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="11" t="s">
-        <v>116</v>
+      <c r="A48" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="11" t="s">
-        <v>192</v>
+      <c r="A51" s="10" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="11" t="s">
-        <v>194</v>
+      <c r="A53" s="10" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="10" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="11" t="s">
-        <v>211</v>
+      <c r="A58" s="10" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="11" t="s">
-        <v>203</v>
+      <c r="A62" s="10" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="11" t="s">
-        <v>205</v>
+      <c r="A64" s="10" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="11" t="s">
-        <v>232</v>
+      <c r="A66" s="10" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="11"/>
+      <c r="A67" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3070,7 +3112,7 @@
     <hyperlink ref="A12" r:id="rId9" display="https://data.sagepub.com/dataset?view=AA8BXQAAgACKAQAAAAAAAAAA3_zMslwIJ8Ve1X%24GDX5KBB%24SwKQSy5xtPfKAgk1iG4StZaRIL6l7otnx6yKcdLvzDvLRvCEbO2BAcdhKAW%24i7s_WK0gRx25yGwTupuJj%24PDiDVMl5kS4rPjBCVz_bmizIUiyn7HJ6yS3e2uia0EdeYj3vmuNnLIQ_MVwcEp1ynYZNzgIxL8S8g0648Vvo73UhTi0ruQ4M2s5Mf7tni7LtgA%24KSA82EBnpvLAyjmwgHjn66NHUUuKsb9AFnB26DU" xr:uid="{7B465DAE-86E7-4CDA-8C23-5AFCAE6C2AA1}"/>
     <hyperlink ref="A15" r:id="rId10" display="https://data.sagepub.com/dataset?view=AA8BXQAAgABOAQAAAAAAAAAA3_zMslwIJ8Ve1X%24GGUIAGV%24TYjZIzxCmS77r7PCMzRPQFNWRmSc7Xe%24J3wl4XB85e_G0bbSso_BthsSkYt2Y_cBhTv039t0noqM2LoUjvdFlA1smTQ%24ftDDAvO7J55tcSKp66TE2ofN%247TlCOdt8Qa2jLbZWzfGfOMm0n6H644dRIqB3Q%24w939EIvKSPHyjoY9qcALCeZ0B0_tlyuI0m_4K7fB_6%24Aox" xr:uid="{150426F6-0169-4E39-8039-A4796F513DEC}"/>
     <hyperlink ref="A17" r:id="rId11" display="https://data.sagepub.com/dataset?view=AA8BXQAAgACHAQAAAAAAAAAA3_zMslwIJ8Ve1X%24GGUHw3Odmzo6pdFI67uULl40M53EEjYiDE9hiyjMvO6unHgrMwfehSNdelyw1KLeotWXTuo0pio_9wcCEdrDdFW9AHSlmIOiACzD0A5_AE4LBir5e_Ztd0D3quDL91nqzxiDbqANOAhMYdgjH1Mwx6DveziLCV0ITxz4IvrZ_g6sjZGZN7CSWPEPihV_JrZlrBaKzLIx%2449nSOEwYxJrLGUSB%24ANsJ7QSXU9RaCp%24bpeKEdY0kA" xr:uid="{579B57D4-0379-439A-94C5-07B56BF224FE}"/>
-    <hyperlink ref="A19" r:id="rId12" display="https://data.sagepub.com/dataset?view=AA8BXQAAgABSAQAAAAAAAAAA3_zMslwIJ8Ve1X%24GDY3Fyttm1VQZdFFmM%247X9sRDMaHIEy2ubabGyUEvljDiYFPO5OZ12TlY7HcKhf%24wIthxDZzTK1fHHO2VZgOTmYjQAG7LKCupmqEExb4QLGT_SXAog5sSaYjvwFQmVjiYTrzhOV%24hH0%24QRqz0oiE4OFw5_UMgrDQCOO2CbYIQSmBOlfTcwQtjHtsCD7%24qWwlTjO_iAejiQhesWl7kvd4ukihJuNt0G1Py" xr:uid="{04EB1B0C-289B-4CBD-AEDE-CE1F69807EB3}"/>
+    <hyperlink ref="A19" r:id="rId12" xr:uid="{04EB1B0C-289B-4CBD-AEDE-CE1F69807EB3}"/>
     <hyperlink ref="A23" r:id="rId13" display="https://data.sagepub.com/dataset?view=AA8BXQAAgABeAQAAAAAAAAAA3_zMslwIJ8Ve1X%24GBLJ59KRaaIlI5gp8ZXcRr0y%24O9jZd2BOrTWTsPQLtjWLM7xxVwRrxqNWFVR68sMfdb0Jz%2408lmd44MPR_Cs70KGn1UPxqlpVvs0cIqeYuNPZkM9FdB2HESmzcFZ46kQU0HoauTg%243ASN8XQXOwPQX88LU930vJYtjHaDDopVu3vs0kYNMKaBbTinQz31P_ZuZVPemgtW9PamPT%24HvCoCi6KO5zu1GmQ9hu0NQ%24oT12TCntBfzg" xr:uid="{03BE96CB-F33F-4CCA-942A-2472A9274117}"/>
     <hyperlink ref="A25" r:id="rId14" display="https://data.sagepub.com/dataset?view=AA8BXQAAgADBAQAAAAAAAAAA3_zMslwIJ8Ve1X%24GGUIAGV%24%24OXmoKwv%248h9BQL65ABBTb0xJuSo7_x7g%24ACos5uUhPbJezdPIN5dzGX%24hnJzwpggzmNXjn5nsrAAw89RGEd0gFRxxJn0gYwoKMcLTDrvEDAVKPeQ88BhZnc6bKBD9bpWd1EuObzun596%24QWNZ30vSttIgq_JITh42OZbThT2barVLKCi_MwlG7rcfxXf9_SytLxdnuDrlqdhd%24xrTbm08PiV65oFubMy9g1WAGNUdzECI1YwjQYnyUsNqXEA" xr:uid="{8C6F66D0-519F-43E2-8C8F-A5B3AAE0671F}"/>
     <hyperlink ref="A26" r:id="rId15" display="https://data.sagepub.com/dataset?view=AA8BXQAAgAC0AQAAAAAAAAAA3_zMslwIJ8Ve1X%24GGUIAGV%24%24Mui4Kw%24IkmsyBLUK5lyAh7fFhx6B64FOqeUxIhLQZ0uFXu1vHPm0pxHQ8gQ3v1N3EjF73LdtRk1Jerc7iS_mSoCHTKLEuTtV14_26S4OQRwa_owUiIxQ5rC1gsqMn9JZrIFan0gFCS0j42OfTaFMvrG8Oagp4myNDpB5KtZjuN_2X5GXSJSCmCHrKaIZ4grnZ3hCPfJQNk4Kuw9WFcorXNtEzS5S52TChO7nLuaVv2IMf3zO" xr:uid="{8D3E4E19-0AF3-40BC-8D23-79A6E626CB85}"/>

</xml_diff>